<commit_message>
Cucumber Class 4 commit 1
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hrmsTestdata.xlsx
+++ b/src/test/resources/testdata/hrmsTestdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jama\Desktop\Bootcamps\Syntax\SyntaxMavenProject\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jama\Desktop\Bootcamps\Syntax\HRMSCucumber\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75D0FD8-4E58-4F73-B66E-039609481981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893460EF-E71A-4347-817A-C4D22C48E9F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{FB663B37-F28E-4922-8B1A-79EDB7B1DAD9}"/>
   </bookViews>
@@ -87,13 +87,13 @@
     <t>C:\Users\Jama\Pictures\testng-tutorial.png</t>
   </si>
   <si>
-    <t>anasule001234567</t>
-  </si>
-  <si>
-    <t>blakenailya001234567</t>
-  </si>
-  <si>
-    <t>mikeaj001234567</t>
+    <t>anasule0012345678</t>
+  </si>
+  <si>
+    <t>blakenailya0012345678</t>
+  </si>
+  <si>
+    <t>mikeaj0012345678</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,8 +467,8 @@
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>